<commit_message>
Maj journal dev par actualisé
</commit_message>
<xml_diff>
--- a/Documentations/JournalDev.xlsx
+++ b/Documentations/JournalDev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\GroupieTracker_Garrigues_Hugo\GroupieTracker_Garrigues_Hugo\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16287BC8-9606-4A7B-ACDE-EDE73AF16E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FECF37-5D44-475C-93E7-9FF79D116AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Journal De Dev</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Journal DEV réalisé dans le temps que je me suis donné</t>
+  </si>
+  <si>
+    <t>ReadMe.md réalisé dans le temps que je me suis donné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maquette page requêtes faites </t>
   </si>
 </sst>
 </file>
@@ -352,58 +358,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,134 +703,116 @@
     <col min="5" max="5" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
         <v>44991</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="13" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="24" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
         <v>44992</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="2" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="13" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26"/>
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Dernier push de la documentations
</commit_message>
<xml_diff>
--- a/Documentations/JournalDev.xlsx
+++ b/Documentations/JournalDev.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\GroupieTracker_Garrigues_Hugo\GroupieTracker_Garrigues_Hugo\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FECF37-5D44-475C-93E7-9FF79D116AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8ABA1F-5C15-47D6-B39D-50792A77F59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Journal De Dev</t>
   </si>
@@ -70,6 +70,123 @@
   </si>
   <si>
     <t xml:space="preserve">Maquette page requêtes faites </t>
+  </si>
+  <si>
+    <t>Renseignement sur le golang effectué</t>
+  </si>
+  <si>
+    <t>Ajout et recherche des fonts</t>
+  </si>
+  <si>
+    <t>Update index.html</t>
+  </si>
+  <si>
+    <t>Ajout d'images</t>
+  </si>
+  <si>
+    <t>Ajout vidéos pour index</t>
+  </si>
+  <si>
+    <t>Ajout logos des maisons</t>
+  </si>
+  <si>
+    <t>Déplacements des assets et du CSS</t>
+  </si>
+  <si>
+    <t>Ajout du template protagonist</t>
+  </si>
+  <si>
+    <t>Ajout du template spells</t>
+  </si>
+  <si>
+    <t>Mise a jour index et css</t>
+  </si>
+  <si>
+    <t>Création du template ron</t>
+  </si>
+  <si>
+    <t>Création du template hermione</t>
+  </si>
+  <si>
+    <t>Création du template harry</t>
+  </si>
+  <si>
+    <t>Création du template character</t>
+  </si>
+  <si>
+    <t>Création du template show characters</t>
+  </si>
+  <si>
+    <t>Création de la page html show characters</t>
+  </si>
+  <si>
+    <t>Création du css show characters</t>
+  </si>
+  <si>
+    <t>Supression du template harry, ron, hermione</t>
+  </si>
+  <si>
+    <t>Amélioration du css show characters</t>
+  </si>
+  <si>
+    <t>17-19-mars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amélioration du css </t>
+  </si>
+  <si>
+    <t>Fonts harry potter recherché, police lumos, police montserrat, police HarryP</t>
+  </si>
+  <si>
+    <t>Amélioration de la page index.html, ajout de l'emplacement pour la vidéo</t>
+  </si>
+  <si>
+    <t>Images pour la navbar</t>
+  </si>
+  <si>
+    <t>Vidéos Harry Potter pour fond de la page index.html</t>
+  </si>
+  <si>
+    <t>Logos des maisons trouvé pour mettre sur la page index.html et acceder aux pages des maisons</t>
+  </si>
+  <si>
+    <t>Template charcter qui demande a l'utilisateur de choisir la maison qu'il souhaite et cela lui affiche tout les personnage</t>
+  </si>
+  <si>
+    <t>Déplacement des assets qui faisaient, que le css ne s'acutalisé pas en localhost</t>
+  </si>
+  <si>
+    <t>Template protagonist ajouté qui montre les informations de Harry, ron hermione</t>
+  </si>
+  <si>
+    <t>Template spells ajouté qui permet de voir tout les sorts d'Harry Potter</t>
+  </si>
+  <si>
+    <t>Mise a jour d'index html</t>
+  </si>
+  <si>
+    <t>Création du template ron qui montre toutes les informations de ron</t>
+  </si>
+  <si>
+    <t>Création du template harry qui montre toutes les informations de harry</t>
+  </si>
+  <si>
+    <t>Création du template hermione qui montre toutes les informations de hermione</t>
+  </si>
+  <si>
+    <t>Création du template show character qui fais en sorte que quand on cherche n'importe quelle personnage cela affiche toutes ses informations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page HTML qui mets une grande carte avec les informations du personnage séléctioné </t>
+  </si>
+  <si>
+    <t>Page css qui met la carte css au milieu</t>
+  </si>
+  <si>
+    <t>Supression de ces templates car jugée inutile</t>
+  </si>
+  <si>
+    <t>Amélioration du CSS de toutes les pages</t>
   </si>
 </sst>
 </file>
@@ -106,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -223,7 +340,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -241,7 +358,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -256,9 +373,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -268,6 +383,58 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -275,17 +442,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -293,56 +449,17 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -350,6 +467,45 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -358,29 +514,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -390,25 +535,58 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,138 +867,368 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="70" customWidth="1"/>
+    <col min="5" max="5" width="120.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="35">
         <v>44991</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="14" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="24">
+      <c r="A6" s="29">
         <v>44992</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="20">
+        <v>44997</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="17"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="10"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28"/>
+      <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <v>44996</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
+        <v>44997</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
+        <v>44998</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
+        <v>44999</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="19">
+        <v>45001</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="23"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="16"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="12">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A22:A24"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A27" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>